<commit_message>
Fix units on household emissions.
</commit_message>
<xml_diff>
--- a/chapters/ch06-CarbonIntensity/datasets/US-Carbon-Emissions.xlsx
+++ b/chapters/ch06-CarbonIntensity/datasets/US-Carbon-Emissions.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/MCBook2021/chapters/ch06-CarbonIntensity/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch06-CarbonIntensity/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA60C3-7B70-E346-B93C-412AF6C2472E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45119B47-6151-0F41-8664-7F23351F31B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20740" yWindow="6540" windowWidth="28040" windowHeight="17440" xr2:uid="{99AEB9AF-F832-1A42-B8E0-A6266B18C0E3}"/>
+    <workbookView xWindow="7800" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{99AEB9AF-F832-1A42-B8E0-A6266B18C0E3}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="3" r:id="rId1"/>
     <sheet name="US elect cons 2018" sheetId="1" r:id="rId2"/>
     <sheet name="CO2 emissions" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,22 +56,22 @@
     <t>Elect cons [quads]</t>
   </si>
   <si>
-    <t>CO2 emiss [tonnes]</t>
-  </si>
-  <si>
     <t>Sector</t>
   </si>
   <si>
     <t>Elect gen</t>
   </si>
   <si>
-    <t>CO2 emiss elect alloc[tonnes]</t>
-  </si>
-  <si>
-    <t>CO2 emissions allocated [tonnes]</t>
-  </si>
-  <si>
     <t>CO2 share</t>
+  </si>
+  <si>
+    <t>CO2 emiss [million tonnes]</t>
+  </si>
+  <si>
+    <t>CO2 emiss elect alloc[million tonnes]</t>
+  </si>
+  <si>
+    <t>CO2 emissions allocated [million tonnes]</t>
   </si>
 </sst>
 </file>
@@ -426,10 +426,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
@@ -438,7 +441,7 @@
       </c>
       <c r="B1" t="str">
         <f>'CO2 emissions'!D1</f>
-        <v>CO2 emissions allocated [tonnes]</v>
+        <v>CO2 emissions allocated [million tonnes]</v>
       </c>
       <c r="C1" t="str">
         <f>'CO2 emissions'!E1</f>
@@ -511,14 +514,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -585,26 +588,26 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -689,7 +692,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>1764</v>

</xml_diff>